<commit_message>
added packages text file
</commit_message>
<xml_diff>
--- a/r4ds schedule.xlsx
+++ b/r4ds schedule.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dnz-my.sharepoint.com/personal/ben_marmont_dairynz_co_nz/Documents/Documents/R/waikato_r4ds_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{026BD8BE-136F-4E31-8F89-FB9C4EC303FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{026BD8BE-136F-4E31-8F89-FB9C4EC303FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2468D059-6EF1-4418-BE47-86B61E4648E5}"/>
   <bookViews>
-    <workbookView xWindow="-10140" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{FE4A9294-5F9F-48DC-8AE2-2E172E3DD284}"/>
+    <workbookView xWindow="-25320" yWindow="75" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{FE4A9294-5F9F-48DC-8AE2-2E172E3DD284}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -114,12 +115,129 @@
   </si>
   <si>
     <t>Week</t>
+  </si>
+  <si>
+    <t>arrow,</t>
+  </si>
+  <si>
+    <t>babynames,</t>
+  </si>
+  <si>
+    <t>curl (&gt;= 5.0.0),</t>
+  </si>
+  <si>
+    <t>dplyr,</t>
+  </si>
+  <si>
+    <t>duckdb,</t>
+  </si>
+  <si>
+    <t>gapminder,</t>
+  </si>
+  <si>
+    <t>ggrepel,</t>
+  </si>
+  <si>
+    <t>ggridges,</t>
+  </si>
+  <si>
+    <t>ggthemes,</t>
+  </si>
+  <si>
+    <t>hexbin,</t>
+  </si>
+  <si>
+    <t>janitor,</t>
+  </si>
+  <si>
+    <t>Lahman,</t>
+  </si>
+  <si>
+    <t>leaflet,</t>
+  </si>
+  <si>
+    <t>maps,</t>
+  </si>
+  <si>
+    <t>nycflights13,</t>
+  </si>
+  <si>
+    <t>openxlsx,</t>
+  </si>
+  <si>
+    <t>palmerpenguins,</t>
+  </si>
+  <si>
+    <t>repurrrsive (&gt;= 1.1.0),</t>
+  </si>
+  <si>
+    <t>tidymodels,</t>
+  </si>
+  <si>
+    <t>tidyverse,</t>
+  </si>
+  <si>
+    <t>writexl,</t>
+  </si>
+  <si>
+    <t>downlit,</t>
+  </si>
+  <si>
+    <t>jpeg,</t>
+  </si>
+  <si>
+    <t>knitr,</t>
+  </si>
+  <si>
+    <t>rmarkdown,</t>
+  </si>
+  <si>
+    <t>sessioninfo,</t>
+  </si>
+  <si>
+    <t>xml2,</t>
+  </si>
+  <si>
+    <t>gt,</t>
+  </si>
+  <si>
+    <t>shiny,</t>
+  </si>
+  <si>
+    <t>readxl,</t>
+  </si>
+  <si>
+    <t>dbplyr,</t>
+  </si>
+  <si>
+    <t>DBI,</t>
+  </si>
+  <si>
+    <t>patchwork,</t>
+  </si>
+  <si>
+    <t>repurrrsive,</t>
+  </si>
+  <si>
+    <t>jsonlite,</t>
+  </si>
+  <si>
+    <t>rvest,</t>
+  </si>
+  <si>
+    <t>magick,</t>
+  </si>
+  <si>
+    <t>webshot2,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="&quot;&quot;&quot;@&quot;&quot;&quot;"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -289,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -363,6 +481,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8D1657-6952-40A4-812C-1865D52ABA57}">
   <dimension ref="B3:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:M20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,6 +1424,212 @@
     <mergeCell ref="J5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52841E11-D468-4F91-947D-689CC4699BE3}">
+  <dimension ref="A1:A38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A1:A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>